<commit_message>
Aaand I didn't commit and can't tell what I've done at that moment...
</commit_message>
<xml_diff>
--- a/data/abundance_surveys/Recap_sources_surveys.xlsx
+++ b/data/abundance_surveys/Recap_sources_surveys.xlsx
@@ -1,26 +1,38 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20379"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{050B0C51-CF6A-4BC6-B097-94C9D2EB9A6E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5871D874-5F0E-418E-A6B9-4A99326561E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Feuil1!$A$1:$N$42</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="208">
   <si>
     <t>Area</t>
   </si>
@@ -569,9 +581,6 @@
   </si>
   <si>
     <t>Mannocci et al 2013</t>
-  </si>
-  <si>
-    <t>163010+110594</t>
   </si>
   <si>
     <t>design-based + geostatistics</t>
@@ -1044,12 +1053,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:N42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="11900" topLeftCell="J1"/>
-      <selection activeCell="F13" sqref="F13"/>
-      <selection pane="topRight" activeCell="K9" sqref="K9"/>
+      <pane xSplit="11900" topLeftCell="J1" activePane="topRight"/>
+      <selection activeCell="G7" sqref="G7"/>
+      <selection pane="topRight" activeCell="K8" sqref="K8:L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1194,7 +1204,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A4" s="18"/>
       <c r="B4" t="s">
         <v>23</v>
@@ -1361,26 +1371,27 @@
       <c r="F8" t="s">
         <v>182</v>
       </c>
-      <c r="G8" t="s">
-        <v>183</v>
+      <c r="G8">
+        <f>163010+110594</f>
+        <v>273604</v>
       </c>
       <c r="H8" t="s">
         <v>26</v>
       </c>
       <c r="I8" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="K8" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="L8" s="1" t="s">
-        <v>21</v>
+      <c r="L8" s="2" t="s">
+        <v>43</v>
       </c>
       <c r="N8" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A9" s="18"/>
       <c r="B9" t="s">
         <v>38</v>
@@ -1419,7 +1430,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A10" s="18"/>
       <c r="B10" t="s">
         <v>38</v>
@@ -1494,13 +1505,13 @@
         <v>21</v>
       </c>
       <c r="M11" t="s">
+        <v>191</v>
+      </c>
+      <c r="N11" t="s">
         <v>192</v>
       </c>
-      <c r="N11" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
+    </row>
+    <row r="12" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A12" s="18"/>
       <c r="B12" t="s">
         <v>50</v>
@@ -1515,7 +1526,7 @@
         <v>2011</v>
       </c>
       <c r="F12" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="G12">
         <v>451985</v>
@@ -1539,19 +1550,19 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:14" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A13" s="18"/>
       <c r="B13" t="s">
+        <v>202</v>
+      </c>
+      <c r="D13" t="s">
         <v>203</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E13" t="s">
         <v>204</v>
       </c>
-      <c r="E13" t="s">
+      <c r="F13" t="s">
         <v>205</v>
-      </c>
-      <c r="F13" t="s">
-        <v>206</v>
       </c>
       <c r="G13">
         <v>43449</v>
@@ -1563,10 +1574,10 @@
         <v>43</v>
       </c>
       <c r="N13" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.35">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" s="5" customFormat="1" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A14" s="18"/>
       <c r="B14" s="5" t="s">
         <v>61</v>
@@ -1590,10 +1601,10 @@
         <v>43</v>
       </c>
       <c r="N14" s="5" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.35">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" s="5" customFormat="1" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A15" s="18"/>
       <c r="B15" s="5" t="s">
         <v>139</v>
@@ -1623,7 +1634,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="16" spans="1:14" s="5" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:14" s="5" customFormat="1" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A16" s="19"/>
       <c r="B16" s="3" t="s">
         <v>168</v>
@@ -1696,7 +1707,7 @@
       </c>
       <c r="N17" s="5"/>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A18" s="18"/>
       <c r="B18" s="3" t="s">
         <v>85</v>
@@ -1732,7 +1743,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="19" spans="1:14" s="7" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:14" s="7" customFormat="1" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A19" s="19"/>
       <c r="B19" s="6" t="s">
         <v>91</v>
@@ -1765,7 +1776,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="20" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:14" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A20" s="18" t="s">
         <v>63</v>
       </c>
@@ -1797,7 +1808,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A21" s="18"/>
       <c r="B21" s="3" t="s">
         <v>68</v>
@@ -1863,7 +1874,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="23" spans="1:14" s="7" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:14" s="7" customFormat="1" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A23" s="19"/>
       <c r="B23" s="6" t="s">
         <v>173</v>
@@ -1888,10 +1899,10 @@
         <v>43</v>
       </c>
       <c r="N23" s="7" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.35">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A24" s="18" t="s">
         <v>94</v>
       </c>
@@ -1926,7 +1937,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A25" s="18"/>
       <c r="B25" s="3" t="s">
         <v>95</v>
@@ -1953,7 +1964,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A26" s="18"/>
       <c r="B26" s="3" t="s">
         <v>109</v>
@@ -1983,10 +1994,10 @@
         <v>43</v>
       </c>
       <c r="N26" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.35">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A27" s="18"/>
       <c r="B27" s="3" t="s">
         <v>109</v>
@@ -2016,7 +2027,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A28" s="18"/>
       <c r="B28" s="3" t="s">
         <v>119</v>
@@ -2043,7 +2054,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A29" s="18"/>
       <c r="B29" s="3" t="s">
         <v>117</v>
@@ -2073,7 +2084,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A30" s="18"/>
       <c r="B30" s="3" t="s">
         <v>117</v>
@@ -2133,10 +2144,10 @@
         <v>21</v>
       </c>
       <c r="N31" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="32" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.35">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A32" s="18"/>
       <c r="B32" s="3" t="s">
         <v>132</v>
@@ -2163,20 +2174,20 @@
         <v>135</v>
       </c>
     </row>
-    <row r="33" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:14" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A33" s="18"/>
       <c r="B33" s="3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D33" s="3"/>
       <c r="E33" s="5" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="G33" s="5">
         <v>2447635</v>
@@ -2185,7 +2196,7 @@
         <v>27</v>
       </c>
       <c r="I33" s="3" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="K33" s="4" t="s">
         <v>21</v>
@@ -2194,23 +2205,23 @@
         <v>43</v>
       </c>
       <c r="N33" s="3" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="34" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A34" s="18"/>
       <c r="B34" s="3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D34" s="3"/>
       <c r="E34" s="3" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="G34" s="5">
         <v>2447635</v>
@@ -2228,7 +2239,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A35" s="18"/>
       <c r="B35" s="3" t="s">
         <v>144</v>
@@ -2258,7 +2269,7 @@
     <row r="36" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A36" s="18"/>
       <c r="B36" s="3" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C36" t="s">
         <v>33</v>
@@ -2294,7 +2305,7 @@
     <row r="37" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A37" s="18"/>
       <c r="B37" s="3" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C37" t="s">
         <v>33</v>
@@ -2333,7 +2344,7 @@
     <row r="38" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A38" s="18"/>
       <c r="B38" s="3" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C38" t="s">
         <v>33</v>
@@ -2363,7 +2374,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A39" s="18"/>
       <c r="B39" s="3" t="s">
         <v>151</v>
@@ -2390,7 +2401,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="40" spans="1:14" s="7" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:14" s="7" customFormat="1" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A40" s="19"/>
       <c r="B40" s="6" t="s">
         <v>151</v>
@@ -2420,10 +2431,10 @@
         <v>43</v>
       </c>
       <c r="N40" s="7" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="41" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.35">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A41" s="17" t="s">
         <v>158</v>
       </c>
@@ -2455,7 +2466,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="42" spans="1:14" s="7" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:14" s="7" customFormat="1" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A42" s="19"/>
       <c r="B42" s="6" t="s">
         <v>160</v>
@@ -2489,6 +2500,13 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:N42" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <filterColumn colId="11">
+      <filters>
+        <filter val="yes"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <mergeCells count="5">
     <mergeCell ref="A17:A19"/>
     <mergeCell ref="A24:A40"/>

</xml_diff>